<commit_message>
Added new test project
</commit_message>
<xml_diff>
--- a/dataTesting.xlsx
+++ b/dataTesting.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Testing\testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\OISP\Software testing\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EE55660-9695-448E-92E9-51A1C82D15AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3E07517-EAD4-4AA2-81B4-D980C37DF029}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3980" yWindow="4100" windowWidth="19200" windowHeight="11180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
+    <sheet name="Signup" sheetId="2" r:id="rId2"/>
+    <sheet name="Search" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>username</t>
   </si>
@@ -37,16 +39,63 @@
   </si>
   <si>
     <t>abcd</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>account</t>
+  </si>
+  <si>
+    <t>day</t>
+  </si>
+  <si>
+    <t>month</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>0127775199</t>
+  </si>
+  <si>
+    <t>aa@gmail.com</t>
+  </si>
+  <si>
+    <t>aa@bb</t>
+  </si>
+  <si>
+    <t>0937746383</t>
+  </si>
+  <si>
+    <t>Phước Nguyễn</t>
+  </si>
+  <si>
+    <t>Male</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -69,13 +118,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -356,13 +410,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -370,7 +424,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -378,7 +432,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -389,4 +443,115 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31A0257A-159E-4424-90FD-8475D7F4B76B}">
+  <dimension ref="A1:H8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="12.54296875" customWidth="1"/>
+    <col min="2" max="2" width="15.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2">
+        <v>25</v>
+      </c>
+      <c r="F2">
+        <v>8</v>
+      </c>
+      <c r="G2">
+        <v>2002</v>
+      </c>
+      <c r="H2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>8493777199</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>937775199</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>1237775199</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B7" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B8" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B7" r:id="rId1" display="aa@" xr:uid="{61F7A90F-7F5F-41EF-AA0A-15F6F3F7E61E}"/>
+    <hyperlink ref="B8" r:id="rId2" xr:uid="{1E25485A-D817-4249-B0F1-519148EE9904}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BCEB427-AA86-4933-9E06-2C7CCC656FC9}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add Login and Tracking order
</commit_message>
<xml_diff>
--- a/dataTesting.xlsx
+++ b/dataTesting.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Testing\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EE55660-9695-448E-92E9-51A1C82D15AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7423F59-FF54-48DC-8528-8574591F87D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3980" yWindow="4100" windowWidth="19200" windowHeight="11180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="15466" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
+    <sheet name="TrackingOrder" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="10">
   <si>
     <t>username</t>
   </si>
@@ -33,20 +34,46 @@
     <t>password</t>
   </si>
   <si>
-    <t>abc</t>
-  </si>
-  <si>
-    <t>abcd</t>
+    <t>OrderId</t>
+  </si>
+  <si>
+    <t>Hatemyself@1001@@</t>
+  </si>
+  <si>
+    <t>thuctanphu12@gmail.com</t>
+  </si>
+  <si>
+    <t>123456</t>
+  </si>
+  <si>
+    <t>aaa@bbb</t>
+  </si>
+  <si>
+    <t>03547305</t>
+  </si>
+  <si>
+    <t>thuctanphuaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaa@gmail.com</t>
+  </si>
+  <si>
+    <t>123456789a</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -69,13 +96,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -354,36 +386,133 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <cols>
+    <col min="1" max="1" width="9.76171875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A6" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="B7" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A8">
+        <v>354730579</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{CD6927AF-EEA8-44A5-8BD1-7BE55D2053CD}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{AD146BA8-C377-4F11-B8F0-4260D4E24AF1}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{A42211E5-F73E-4B7F-8549-307926CC1F82}"/>
+    <hyperlink ref="B4" r:id="rId4" xr:uid="{806E08E6-46D5-4D4B-9F8F-8E2F66148336}"/>
+    <hyperlink ref="A5" r:id="rId5" xr:uid="{FD0E97CC-3B27-4638-BACE-8735F9E245FA}"/>
+    <hyperlink ref="B5" r:id="rId6" xr:uid="{149C66EA-1523-4811-8D11-373D854697B6}"/>
+    <hyperlink ref="A6" r:id="rId7" xr:uid="{6F062309-B91E-4157-A6DD-A741702E0D14}"/>
+    <hyperlink ref="B7" r:id="rId8" xr:uid="{26BE3A12-4B4A-4CA6-9BCF-0FD476709FDC}"/>
+    <hyperlink ref="B8" r:id="rId9" xr:uid="{59A373C0-97C8-410C-AD31-9942BC302857}"/>
+    <hyperlink ref="B9" r:id="rId10" xr:uid="{EEFE168A-8727-4253-95AF-02269F03A9C8}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C13B502F-03A6-40A4-8514-914CD1B5F5A4}">
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A2">
+        <v>392921444522425</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A3">
+        <v>440277016458018</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A4">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.5">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.5">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>12321</v>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A5" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Login and Tracking order (#1)
</commit_message>
<xml_diff>
--- a/dataTesting.xlsx
+++ b/dataTesting.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Testing\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EE55660-9695-448E-92E9-51A1C82D15AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7423F59-FF54-48DC-8528-8574591F87D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3980" yWindow="4100" windowWidth="19200" windowHeight="11180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="15466" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
+    <sheet name="TrackingOrder" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="10">
   <si>
     <t>username</t>
   </si>
@@ -33,20 +34,46 @@
     <t>password</t>
   </si>
   <si>
-    <t>abc</t>
-  </si>
-  <si>
-    <t>abcd</t>
+    <t>OrderId</t>
+  </si>
+  <si>
+    <t>Hatemyself@1001@@</t>
+  </si>
+  <si>
+    <t>thuctanphu12@gmail.com</t>
+  </si>
+  <si>
+    <t>123456</t>
+  </si>
+  <si>
+    <t>aaa@bbb</t>
+  </si>
+  <si>
+    <t>03547305</t>
+  </si>
+  <si>
+    <t>thuctanphuaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaa@gmail.com</t>
+  </si>
+  <si>
+    <t>123456789a</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -69,13 +96,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -354,36 +386,133 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <cols>
+    <col min="1" max="1" width="9.76171875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A6" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="B7" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A8">
+        <v>354730579</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{CD6927AF-EEA8-44A5-8BD1-7BE55D2053CD}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{AD146BA8-C377-4F11-B8F0-4260D4E24AF1}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{A42211E5-F73E-4B7F-8549-307926CC1F82}"/>
+    <hyperlink ref="B4" r:id="rId4" xr:uid="{806E08E6-46D5-4D4B-9F8F-8E2F66148336}"/>
+    <hyperlink ref="A5" r:id="rId5" xr:uid="{FD0E97CC-3B27-4638-BACE-8735F9E245FA}"/>
+    <hyperlink ref="B5" r:id="rId6" xr:uid="{149C66EA-1523-4811-8D11-373D854697B6}"/>
+    <hyperlink ref="A6" r:id="rId7" xr:uid="{6F062309-B91E-4157-A6DD-A741702E0D14}"/>
+    <hyperlink ref="B7" r:id="rId8" xr:uid="{26BE3A12-4B4A-4CA6-9BCF-0FD476709FDC}"/>
+    <hyperlink ref="B8" r:id="rId9" xr:uid="{59A373C0-97C8-410C-AD31-9942BC302857}"/>
+    <hyperlink ref="B9" r:id="rId10" xr:uid="{EEFE168A-8727-4253-95AF-02269F03A9C8}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C13B502F-03A6-40A4-8514-914CD1B5F5A4}">
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A2">
+        <v>392921444522425</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A3">
+        <v>440277016458018</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A4">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.5">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.5">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>12321</v>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A5" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: add test for add voucher feature
</commit_message>
<xml_diff>
--- a/dataTesting.xlsx
+++ b/dataTesting.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11116"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Testing\testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/congdat/Development/Testing#3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7423F59-FF54-48DC-8528-8574591F87D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BE2EB85-D995-594B-8193-616F4403EB4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="15466" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="25780" windowHeight="15460" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
     <sheet name="TrackingOrder" sheetId="2" r:id="rId2"/>
+    <sheet name="AddVoucher" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
   <si>
     <t>username</t>
   </si>
@@ -56,6 +57,24 @@
   </si>
   <si>
     <t>123456789a</t>
+  </si>
+  <si>
+    <t>Voucher</t>
+  </si>
+  <si>
+    <t>Output</t>
+  </si>
+  <si>
+    <t>LAZADA123</t>
+  </si>
+  <si>
+    <t>Sorry, this voucher is not valid. Please check for any typing errors.</t>
+  </si>
+  <si>
+    <t>GIATOT123</t>
+  </si>
+  <si>
+    <t>LAZADANEWYEAR123</t>
   </si>
 </sst>
 </file>
@@ -392,12 +411,12 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.76171875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -405,7 +424,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -413,7 +432,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -421,7 +440,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -429,7 +448,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
@@ -437,17 +456,17 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>354730579</v>
       </c>
@@ -455,7 +474,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -484,35 +503,85 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C13B502F-03A6-40A4-8514-914CD1B5F5A4}">
   <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>392921444522425</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>440277016458018</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6847CE83-3F2A-894C-B197-8091D1E2B7C5}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="49.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: test signup and search
</commit_message>
<xml_diff>
--- a/dataTesting.xlsx
+++ b/dataTesting.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\OISP\Software testing\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3E07517-EAD4-4AA2-81B4-D980C37DF029}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{660A1D1E-784C-44FC-AA39-31C774224512}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="27">
   <si>
     <t>username</t>
   </si>
@@ -50,18 +50,6 @@
     <t>account</t>
   </si>
   <si>
-    <t>day</t>
-  </si>
-  <si>
-    <t>month</t>
-  </si>
-  <si>
-    <t>year</t>
-  </si>
-  <si>
-    <t>gender</t>
-  </si>
-  <si>
     <t>0127775199</t>
   </si>
   <si>
@@ -77,7 +65,49 @@
     <t>Phước Nguyễn</t>
   </si>
   <si>
-    <t>Male</t>
+    <t>#Sora2508</t>
+  </si>
+  <si>
+    <t>failed at</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>a..a@gmail.com</t>
+  </si>
+  <si>
+    <t>#Sors 2508</t>
+  </si>
+  <si>
+    <t>&amp;^&amp;^#@&amp;hdad</t>
+  </si>
+  <si>
+    <t>query</t>
+  </si>
+  <si>
+    <t>have result</t>
+  </si>
+  <si>
+    <t>tai nghe dareu eh416</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>tai nghr</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>empty</t>
+  </si>
+  <si>
+    <t>ta nghr dareu eh4671</t>
+  </si>
+  <si>
+    <t>234234sfsddfs423</t>
   </si>
 </sst>
 </file>
@@ -122,11 +152,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" quotePrefix="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -447,111 +478,238 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31A0257A-159E-4424-90FD-8475D7F4B76B}">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.54296875" customWidth="1"/>
-    <col min="2" max="2" width="15.26953125" customWidth="1"/>
+    <col min="2" max="2" width="12.54296875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="15.26953125" customWidth="1"/>
+    <col min="5" max="5" width="15.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="3">
+        <v>84937775199</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="3">
+        <v>937775199</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3">
+        <v>1237775199</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F1" t="s">
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G1" t="s">
+      <c r="D7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="D8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E2">
-        <v>25</v>
-      </c>
-      <c r="F2">
-        <v>8</v>
-      </c>
-      <c r="G2">
-        <v>2002</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="D9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <v>8493777199</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>937775199</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5">
-        <v>1237775199</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B7" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B8" s="2" t="s">
-        <v>13</v>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B7" r:id="rId1" display="aa@" xr:uid="{61F7A90F-7F5F-41EF-AA0A-15F6F3F7E61E}"/>
-    <hyperlink ref="B8" r:id="rId2" xr:uid="{1E25485A-D817-4249-B0F1-519148EE9904}"/>
+    <hyperlink ref="C7" r:id="rId1" display="aa@" xr:uid="{61F7A90F-7F5F-41EF-AA0A-15F6F3F7E61E}"/>
+    <hyperlink ref="C8" r:id="rId2" xr:uid="{1E25485A-D817-4249-B0F1-519148EE9904}"/>
+    <hyperlink ref="C9" r:id="rId3" xr:uid="{D7C79134-18DA-4BE2-AE94-816458CA01FE}"/>
+    <hyperlink ref="E11" r:id="rId4" xr:uid="{6618DD33-7F6A-472E-BF0F-5845D4BFD05E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="B2 B6" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BCEB427-AA86-4933-9E06-2C7CCC656FC9}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="11" customWidth="1"/>
+    <col min="2" max="2" width="21.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Sign up & search (#3)
* Added new test project

* feat: test signup and search

* style: clear the print code

* fix: remove read data cache
</commit_message>
<xml_diff>
--- a/dataTesting.xlsx
+++ b/dataTesting.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/congdat/Development/Testing#3/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\OISP\Software testing\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BE2EB85-D995-594B-8193-616F4403EB4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{660A1D1E-784C-44FC-AA39-31C774224512}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="25780" windowHeight="15460" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
-    <sheet name="TrackingOrder" sheetId="2" r:id="rId2"/>
-    <sheet name="AddVoucher" sheetId="3" r:id="rId3"/>
+    <sheet name="Signup" sheetId="2" r:id="rId2"/>
+    <sheet name="Search" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="27">
   <si>
     <t>username</t>
   </si>
@@ -35,46 +35,79 @@
     <t>password</t>
   </si>
   <si>
-    <t>OrderId</t>
-  </si>
-  <si>
-    <t>Hatemyself@1001@@</t>
-  </si>
-  <si>
-    <t>thuctanphu12@gmail.com</t>
-  </si>
-  <si>
-    <t>123456</t>
-  </si>
-  <si>
-    <t>aaa@bbb</t>
-  </si>
-  <si>
-    <t>03547305</t>
-  </si>
-  <si>
-    <t>thuctanphuaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaa@gmail.com</t>
-  </si>
-  <si>
-    <t>123456789a</t>
-  </si>
-  <si>
-    <t>Voucher</t>
-  </si>
-  <si>
-    <t>Output</t>
-  </si>
-  <si>
-    <t>LAZADA123</t>
-  </si>
-  <si>
-    <t>Sorry, this voucher is not valid. Please check for any typing errors.</t>
-  </si>
-  <si>
-    <t>GIATOT123</t>
-  </si>
-  <si>
-    <t>LAZADANEWYEAR123</t>
+    <t>abc</t>
+  </si>
+  <si>
+    <t>abcd</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>account</t>
+  </si>
+  <si>
+    <t>0127775199</t>
+  </si>
+  <si>
+    <t>aa@gmail.com</t>
+  </si>
+  <si>
+    <t>aa@bb</t>
+  </si>
+  <si>
+    <t>0937746383</t>
+  </si>
+  <si>
+    <t>Phước Nguyễn</t>
+  </si>
+  <si>
+    <t>#Sora2508</t>
+  </si>
+  <si>
+    <t>failed at</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>a..a@gmail.com</t>
+  </si>
+  <si>
+    <t>#Sors 2508</t>
+  </si>
+  <si>
+    <t>&amp;^&amp;^#@&amp;hdad</t>
+  </si>
+  <si>
+    <t>query</t>
+  </si>
+  <si>
+    <t>have result</t>
+  </si>
+  <si>
+    <t>tai nghe dareu eh416</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>tai nghr</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>empty</t>
+  </si>
+  <si>
+    <t>ta nghr dareu eh4671</t>
+  </si>
+  <si>
+    <t>234234sfsddfs423</t>
   </si>
 </sst>
 </file>
@@ -119,11 +152,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" quotePrefix="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -405,18 +439,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="9.83203125" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -424,164 +455,258 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="2" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B7" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>354730579</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>3</v>
+      <c r="B3">
+        <v>12321</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{CD6927AF-EEA8-44A5-8BD1-7BE55D2053CD}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{AD146BA8-C377-4F11-B8F0-4260D4E24AF1}"/>
-    <hyperlink ref="A4" r:id="rId3" xr:uid="{A42211E5-F73E-4B7F-8549-307926CC1F82}"/>
-    <hyperlink ref="B4" r:id="rId4" xr:uid="{806E08E6-46D5-4D4B-9F8F-8E2F66148336}"/>
-    <hyperlink ref="A5" r:id="rId5" xr:uid="{FD0E97CC-3B27-4638-BACE-8735F9E245FA}"/>
-    <hyperlink ref="B5" r:id="rId6" xr:uid="{149C66EA-1523-4811-8D11-373D854697B6}"/>
-    <hyperlink ref="A6" r:id="rId7" xr:uid="{6F062309-B91E-4157-A6DD-A741702E0D14}"/>
-    <hyperlink ref="B7" r:id="rId8" xr:uid="{26BE3A12-4B4A-4CA6-9BCF-0FD476709FDC}"/>
-    <hyperlink ref="B8" r:id="rId9" xr:uid="{59A373C0-97C8-410C-AD31-9942BC302857}"/>
-    <hyperlink ref="B9" r:id="rId10" xr:uid="{EEFE168A-8727-4253-95AF-02269F03A9C8}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C13B502F-03A6-40A4-8514-914CD1B5F5A4}">
-  <dimension ref="A1:A5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31A0257A-159E-4424-90FD-8475D7F4B76B}">
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="12.54296875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="15.26953125" customWidth="1"/>
+    <col min="5" max="5" width="15.81640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>392921444522425</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>440277016458018</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4">
+        <v>13</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="3">
+        <v>84937775199</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="3">
+        <v>937775199</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3">
+        <v>1237775199</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="D8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C7" r:id="rId1" display="aa@" xr:uid="{61F7A90F-7F5F-41EF-AA0A-15F6F3F7E61E}"/>
+    <hyperlink ref="C8" r:id="rId2" xr:uid="{1E25485A-D817-4249-B0F1-519148EE9904}"/>
+    <hyperlink ref="C9" r:id="rId3" xr:uid="{D7C79134-18DA-4BE2-AE94-816458CA01FE}"/>
+    <hyperlink ref="E11" r:id="rId4" xr:uid="{6618DD33-7F6A-472E-BF0F-5845D4BFD05E}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="B2 B6" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6847CE83-3F2A-894C-B197-8091D1E2B7C5}">
-  <dimension ref="A1:B4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BCEB427-AA86-4933-9E06-2C7CCC656FC9}">
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="49.6640625" customWidth="1"/>
+    <col min="1" max="1" width="11" customWidth="1"/>
+    <col min="2" max="2" width="21.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>